<commit_message>
Desalin test data changed
</commit_message>
<xml_diff>
--- a/src/test/resources/database/TestData_desalin.xlsx
+++ b/src/test/resources/database/TestData_desalin.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHAMBHU\Downloads\VULCUAN_Cucumber_Framework (1)\VULCUAN_Cucumber_Framework\src\test\resources\database\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0012693-0BF0-489A-B671-AA9E8F55FFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8027E3C3-5A75-433C-B6B0-0EE0B8BBDC15}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21075" windowHeight="6345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocalFT" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Databinding</t>
   </si>
@@ -66,12 +62,6 @@
     <t>fund transfer</t>
   </si>
   <si>
-    <t>5-14-2020</t>
-  </si>
-  <si>
-    <t>60000</t>
-  </si>
-  <si>
     <t>76549876</t>
   </si>
   <si>
@@ -79,6 +69,84 @@
   </si>
   <si>
     <t>Local Transfer</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>TestData_002</t>
+  </si>
+  <si>
+    <t>TestData_003</t>
+  </si>
+  <si>
+    <t>TestData_004</t>
+  </si>
+  <si>
+    <t>TestData_005</t>
+  </si>
+  <si>
+    <t>SBI</t>
+  </si>
+  <si>
+    <t>SCB</t>
+  </si>
+  <si>
+    <t>ICICI</t>
+  </si>
+  <si>
+    <t>IOB</t>
+  </si>
+  <si>
+    <t>kevin</t>
+  </si>
+  <si>
+    <t>mohan</t>
+  </si>
+  <si>
+    <t>sambu</t>
+  </si>
+  <si>
+    <t>gayathri</t>
+  </si>
+  <si>
+    <t>MT104</t>
+  </si>
+  <si>
+    <t>MT105</t>
+  </si>
+  <si>
+    <t>MT106</t>
+  </si>
+  <si>
+    <t>MT107</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>1112</t>
+  </si>
+  <si>
+    <t>1113</t>
+  </si>
+  <si>
+    <t>1114</t>
+  </si>
+  <si>
+    <t>1115</t>
   </si>
 </sst>
 </file>
@@ -117,7 +185,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +480,7 @@
     <col min="4" max="5" width="23.7109375" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -460,21 +528,137 @@
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>25632523</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>23365478</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>23657489</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>1236548</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>